<commit_message>
Updated documentation on SQ19.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14490" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="9" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -856,7 +856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="398">
   <si>
     <t>Step #</t>
   </si>
@@ -1408,9 +1408,6 @@
   </si>
   <si>
     <t>Wait for LI660/LI670/LI680 &lt;= LI660 min/LI670 min/LI680 min then goto 14</t>
-  </si>
-  <si>
-    <t>Waiting for stopping</t>
   </si>
   <si>
     <t>Not isolated</t>
@@ -1580,12 +1577,6 @@
     <t>Cooling</t>
   </si>
   <si>
-    <t>Wait until stoppin state then goto 8</t>
-  </si>
-  <si>
-    <t>Wait in State_Stopping until the valve (CV650/651/652/653) corresponding to selected current lead closes then goto 10</t>
-  </si>
-  <si>
     <t>Wait until FV587 closes then goto 0</t>
   </si>
   <si>
@@ -2200,6 +2191,24 @@
   </si>
   <si>
     <t>Implemented in PLC GERSEMI_2020_02_20</t>
+  </si>
+  <si>
+    <t>Warming-up. Waiting for stop</t>
+  </si>
+  <si>
+    <t>Wait for stop then goto 16</t>
+  </si>
+  <si>
+    <t>Heating-up</t>
+  </si>
+  <si>
+    <t>Wait until stopping state then goto 8</t>
+  </si>
+  <si>
+    <t>End of cooling</t>
+  </si>
+  <si>
+    <t>Wait in State_Stopping until the flows (FT650/651/652/653) corresponding to selected current lead are set to 0 then goto 10</t>
   </si>
 </sst>
 </file>
@@ -2744,6 +2753,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2762,15 +2780,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3520,14 +3529,14 @@
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3536,27 +3545,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3641,7 +3650,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3674,21 +3683,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
-        <v>253</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3760,7 +3769,7 @@
         <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3773,13 +3782,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3790,7 +3799,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3806,7 +3815,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3819,7 +3828,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3830,7 +3839,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3843,10 +3852,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3857,7 +3866,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3873,7 +3882,7 @@
         <v>74</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3889,7 +3898,7 @@
         <v>75</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3905,7 +3914,7 @@
         <v>76</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3921,7 +3930,7 @@
         <v>72</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3940,7 +3949,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3956,7 +3965,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3972,7 +3981,7 @@
         <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3988,7 +3997,7 @@
         <v>68</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4004,7 +4013,7 @@
         <v>63</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4020,7 +4029,7 @@
         <v>65</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4033,10 +4042,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4047,7 +4056,7 @@
         <v>66</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4063,7 +4072,7 @@
         <v>62</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4079,7 +4088,7 @@
         <v>67</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4092,10 +4101,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4106,7 +4115,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4122,7 +4131,7 @@
         <v>69</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4138,7 +4147,7 @@
         <v>70</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4154,27 +4163,27 @@
         <v>66</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B62" s="35" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B64" s="39" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4208,18 +4217,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4275,7 +4284,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4288,7 +4297,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4304,7 +4313,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4320,7 +4329,7 @@
         <v>79</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4336,7 +4345,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4349,10 +4358,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4360,7 +4369,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4371,7 +4380,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4387,7 +4396,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4403,22 +4412,22 @@
         <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4453,11 +4462,11 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -4584,12 +4593,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -4621,21 +4630,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>269</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4688,7 +4697,7 @@
         <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4704,7 +4713,7 @@
         <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4712,10 +4721,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4726,7 +4735,7 @@
         <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4742,7 +4751,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4763,7 +4772,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4797,19 +4806,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="52" t="s">
-        <v>270</v>
-      </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="B3" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
-        <v>274</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4869,7 +4878,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4994,7 +5003,7 @@
         <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5011,7 +5020,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5048,7 +5057,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5082,7 +5091,7 @@
         <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5090,19 +5099,19 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="35" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="35" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5112,37 +5121,37 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="42" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="35" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5177,19 +5186,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5226,7 +5235,7 @@
         <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5242,7 +5251,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5250,10 +5259,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5264,7 +5273,7 @@
         <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5280,7 +5289,7 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5296,7 +5305,7 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5312,12 +5321,12 @@
         <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5351,20 +5360,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5507,20 +5516,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5576,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5589,10 +5598,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
         <v>184</v>
-      </c>
-      <c r="D11" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5608,7 +5617,7 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5621,7 +5630,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
         <v>138</v>
@@ -5640,7 +5649,7 @@
         <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5656,7 +5665,7 @@
         <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -5691,18 +5700,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5755,7 +5764,7 @@
         <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5768,10 +5777,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
         <v>193</v>
-      </c>
-      <c r="D11" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5791,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -5836,116 +5845,116 @@
     </row>
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
-      <c r="B2" s="46" t="s">
-        <v>354</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46"/>
+      <c r="B2" s="49" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
     </row>
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>325</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -5986,16 +5995,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6026,14 +6035,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6062,7 +6071,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6070,7 +6079,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6098,7 +6107,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6107,7 +6116,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6134,7 +6143,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6145,47 +6154,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N9" s="26"/>
-      <c r="O9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="P9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="R9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="S9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="T9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="U9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="V9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="W9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="X9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Y9" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Z9" s="55" t="s">
-        <v>330</v>
+      <c r="O9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="P9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="R9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="S9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="T9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="U9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="V9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="W9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="X9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y9" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z9" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6196,7 +6205,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6207,7 +6216,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6232,7 +6241,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6244,7 +6253,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6268,7 +6277,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6281,7 +6290,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6304,7 +6313,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6318,7 +6327,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6340,7 +6349,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6355,7 +6364,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6376,7 +6385,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6392,7 +6401,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6412,7 +6421,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6429,7 +6438,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6448,7 +6457,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6466,7 +6475,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6484,7 +6493,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6503,10 +6512,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6522,7 +6531,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6542,7 +6551,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6558,7 +6567,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6580,7 +6589,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6594,7 +6603,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6616,7 +6625,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6630,7 +6639,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6653,7 +6662,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6666,7 +6675,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6690,13 +6699,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6706,7 +6715,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6730,13 +6739,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6745,15 +6754,15 @@
       <c r="B25" s="23">
         <v>21</v>
       </c>
-      <c r="C25" s="54" t="s">
-        <v>389</v>
+      <c r="C25" s="46" t="s">
+        <v>386</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
-      <c r="H25" s="55" t="s">
-        <v>330</v>
+      <c r="H25" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6781,19 +6790,19 @@
       <c r="B26" s="23">
         <v>22</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>390</v>
+      <c r="C26" s="46" t="s">
+        <v>387</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
-      <c r="I26" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="J26" s="55" t="s">
-        <v>330</v>
+      <c r="I26" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="J26" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -6819,8 +6828,8 @@
       <c r="B27" s="23">
         <v>23</v>
       </c>
-      <c r="C27" s="54" t="s">
-        <v>391</v>
+      <c r="C27" s="46" t="s">
+        <v>388</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -6830,8 +6839,8 @@
       <c r="I27" s="43"/>
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
-      <c r="L27" s="55" t="s">
-        <v>330</v>
+      <c r="L27" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -6855,8 +6864,8 @@
       <c r="B28" s="23">
         <v>24</v>
       </c>
-      <c r="C28" s="54" t="s">
-        <v>392</v>
+      <c r="C28" s="46" t="s">
+        <v>389</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -6867,30 +6876,30 @@
       <c r="J28" s="43"/>
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
-      <c r="M28" s="55" t="s">
-        <v>330</v>
+      <c r="M28" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="N28" s="43"/>
-      <c r="O28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="P28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="R28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="S28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="T28" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="U28" s="55" t="s">
-        <v>330</v>
+      <c r="O28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="P28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="R28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="S28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="T28" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="U28" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -6905,8 +6914,8 @@
       <c r="B29" s="23">
         <v>25</v>
       </c>
-      <c r="C29" s="54" t="s">
-        <v>393</v>
+      <c r="C29" s="46" t="s">
+        <v>390</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -6927,17 +6936,17 @@
       <c r="T29" s="43"/>
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
-      <c r="W29" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="X29" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Y29" s="55" t="s">
-        <v>330</v>
-      </c>
-      <c r="Z29" s="55" t="s">
-        <v>330</v>
+      <c r="W29" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="X29" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y29" s="47" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z29" s="47" t="s">
+        <v>327</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7076,7 +7085,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7084,7 +7093,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7100,7 +7109,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7114,7 +7123,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7123,7 +7132,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7150,7 +7159,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7162,17 +7171,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7192,7 +7201,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7209,19 +7218,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7393,8 +7402,8 @@
     <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="56" t="s">
-        <v>394</v>
+      <c r="C43" s="48" t="s">
+        <v>391</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7448,11 +7457,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7514,7 +7523,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7616,7 +7625,7 @@
         <v>110</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7632,7 +7641,7 @@
         <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7664,7 +7673,7 @@
         <v>115</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7683,7 +7692,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7715,7 +7724,7 @@
         <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -7747,11 +7756,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7806,10 +7815,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7822,10 +7831,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7841,7 +7850,7 @@
         <v>59</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7854,10 +7863,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7870,10 +7879,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7886,10 +7895,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -7908,8 +7917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7924,11 +7933,11 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
-        <v>214</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7987,10 +7996,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>215</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7999,15 +8008,15 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>218</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8016,15 +8025,15 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>396</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>219</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8038,10 +8047,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -8073,18 +8082,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>386</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>383</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8248,7 +8257,7 @@
         <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8268,7 +8277,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8288,7 +8297,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8350,7 +8359,7 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="40" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -8383,18 +8392,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>289</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8453,7 +8462,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8472,7 +8481,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8491,7 +8500,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8507,7 +8516,7 @@
         <v>150</v>
       </c>
       <c r="D16" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8560,7 +8569,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -8581,7 +8590,7 @@
   <dimension ref="A3:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8593,18 +8602,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8717,7 +8726,7 @@
         <v>161</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8746,10 +8755,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>394</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>393</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8786,7 +8795,7 @@
   <dimension ref="A3:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8798,18 +8807,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8887,7 +8896,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8951,7 +8960,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>392</v>
       </c>
       <c r="D20" t="s">
         <v>163</v>
@@ -8987,18 +8996,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9038,7 +9047,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9051,10 +9060,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9067,10 +9076,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9086,7 +9095,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -9119,18 +9128,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
+      <c r="A3" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9170,7 +9179,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9183,10 +9192,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9199,10 +9208,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9218,7 +9227,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -9596,17 +9605,17 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="35" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
@@ -9982,12 +9991,12 @@
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="37" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="38" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -10354,17 +10363,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -10656,7 +10665,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10690,12 +10699,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -10815,12 +10824,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -10924,7 +10933,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in SQ9. Updated opi.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="9" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="SQ14" sheetId="16" r:id="rId17"/>
     <sheet name="SQ15" sheetId="18" r:id="rId18"/>
     <sheet name="SQ16" sheetId="19" r:id="rId19"/>
-    <sheet name="SQ17" sheetId="20" r:id="rId20"/>
-    <sheet name="SQ18" sheetId="21" r:id="rId21"/>
+    <sheet name="SQ18" sheetId="21" r:id="rId20"/>
+    <sheet name="SQ17" sheetId="20" r:id="rId21"/>
     <sheet name="SQ19" sheetId="22" r:id="rId22"/>
     <sheet name="SQ20" sheetId="23" r:id="rId23"/>
     <sheet name="SQ21" sheetId="24" r:id="rId24"/>
@@ -827,6 +827,30 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="D55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Stopping has been fixed (added) on 2021-04-21</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B62" authorId="0">
       <text>
         <r>
@@ -856,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="400">
   <si>
     <t>Step #</t>
   </si>
@@ -1704,22 +1728,13 @@
     <t>Waiting for LT600 &lt; P_LT600_min then goto 42</t>
   </si>
   <si>
-    <t>Wait for TT602 or TT614 to go below TT Cool-down and CV5203 pERCoUT = 100 and HNOSS comm OK then goto 44</t>
-  </si>
-  <si>
     <t>Wait for level to go below min.</t>
   </si>
   <si>
-    <t>Waiting for LT600 &gt; LT600 Max then goto 46 or ait for changing to PID mode and goto 34</t>
-  </si>
-  <si>
     <t>Waiting for stop Seq9 or Stop Liquefier mode then goto 48 or and Waiting for LT600 &lt; LT600 Min in Intermittent mode and goto 42 or changing to PID mode and goto 34</t>
   </si>
   <si>
     <t>HNOSS comm OK and CV5203 status closed and CV5203 PercOut &lt;= 0 then goto 38</t>
-  </si>
-  <si>
-    <t>Sequence 9: Valve Box cooling &amp; controlling level in 4K tank (Revised 2019-02-25)</t>
   </si>
   <si>
     <t>After Yes goto 8</t>
@@ -2210,12 +2225,27 @@
   <si>
     <t>Wait in State_Stopping until the flows (FT650/651/652/653) corresponding to selected current lead are set to 0 then goto 10</t>
   </si>
+  <si>
+    <t>Updated 2021-02-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting for Yes, then goto 14 (when 2K pumps automatic start-up is active the sequencer program will send Yes cmd in step 5) </t>
+  </si>
+  <si>
+    <t>Sequence 9: Valve Box cooling &amp; controlling level in 4K tank (Revised 2021-04-21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for TT602 or TT614 to go below TT Cool-down and CV5203 pERCoUT = 100 and HNOSS comm OK then goto 44. </t>
+  </si>
+  <si>
+    <t>Waiting for LT600 &gt; LT600 Max then goto 46 or ait for changing to PID mode and goto 34. Can be stopped.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2319,6 +2349,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2968,8 +3011,8 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
-  <autoFilter ref="A5:D34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table13456789101112141520" displayName="Table13456789101112141520" ref="A5:D20" totalsRowShown="0">
+  <autoFilter ref="A5:D20"/>
   <sortState ref="A6:C46">
     <sortCondition ref="A4:A45"/>
   </sortState>
@@ -2984,8 +3027,8 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table13456789101112141520" displayName="Table13456789101112141520" ref="A5:D20" totalsRowShown="0">
-  <autoFilter ref="A5:D20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
+  <autoFilter ref="A5:D34"/>
   <sortState ref="A6:C46">
     <sortCondition ref="A4:A45"/>
   </sortState>
@@ -3536,7 +3579,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3545,27 +3588,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3650,7 +3693,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -3670,8 +3713,8 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3727,7 @@
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="50" t="s">
-        <v>250</v>
+        <v>397</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -4101,13 +4144,13 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>42</v>
       </c>
@@ -4115,7 +4158,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>245</v>
+        <v>398</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4123,7 +4166,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>44</v>
       </c>
@@ -4131,7 +4174,7 @@
         <v>69</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>247</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4147,7 +4190,7 @@
         <v>70</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4163,27 +4206,27 @@
         <v>66</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B62" s="35" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B64" s="39" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -4218,7 +4261,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="50" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -4284,7 +4327,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4297,7 +4340,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4313,7 +4356,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4329,7 +4372,7 @@
         <v>79</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4345,7 +4388,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4358,10 +4401,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4369,7 +4412,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4380,7 +4423,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4396,7 +4439,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4412,22 +4455,22 @@
         <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -4593,12 +4636,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -4631,7 +4674,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -4697,7 +4740,7 @@
         <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4713,7 +4756,7 @@
         <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4721,10 +4764,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4735,7 +4778,7 @@
         <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4751,7 +4794,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4772,7 +4815,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4807,14 +4850,14 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="55" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C3" s="55"/>
       <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="53" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
@@ -4878,7 +4921,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5003,7 +5046,7 @@
         <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5012,7 +5055,7 @@
       </c>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>20</v>
       </c>
@@ -5020,7 +5063,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5029,7 +5072,7 @@
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>22</v>
       </c>
@@ -5046,7 +5089,7 @@
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>24</v>
       </c>
@@ -5057,7 +5100,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5066,7 +5109,7 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>26</v>
       </c>
@@ -5083,7 +5126,7 @@
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>28</v>
       </c>
@@ -5091,67 +5134,67 @@
         <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B39" s="8"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
+        <v>351</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B41" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B42" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B43" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B44" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B45" s="11" t="s">
         <v>355</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
-        <v>356</v>
-      </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
-        <v>358</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5187,7 +5230,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -5235,7 +5278,7 @@
         <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5251,7 +5294,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5259,10 +5302,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5273,7 +5316,7 @@
         <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5289,7 +5332,7 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5305,7 +5348,7 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5321,12 +5364,12 @@
         <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -5846,7 +5889,7 @@
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="49" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
@@ -5878,83 +5921,83 @@
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>322</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>324</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -5995,16 +6038,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6035,14 +6078,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6071,7 +6114,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6079,7 +6122,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6107,7 +6150,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6116,7 +6159,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6137,13 +6180,13 @@
       <c r="AA8" s="26"/>
       <c r="AB8" s="27"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="23">
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6154,47 +6197,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6205,7 +6248,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6216,7 +6259,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6241,7 +6284,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6253,7 +6296,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6277,7 +6320,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6290,7 +6333,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6313,7 +6356,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6327,7 +6370,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6349,7 +6392,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6364,7 +6407,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6385,7 +6428,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6401,7 +6444,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6421,7 +6464,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6438,7 +6481,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6457,7 +6500,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6475,7 +6518,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6493,7 +6536,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6512,10 +6555,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6531,7 +6574,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6551,7 +6594,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6567,7 +6610,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6589,7 +6632,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6603,7 +6646,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6625,7 +6668,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6639,7 +6682,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6662,20 +6705,20 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
       <c r="AA22" s="26"/>
       <c r="AB22" s="27"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="23">
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6699,23 +6742,23 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="23">
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6739,30 +6782,30 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="23">
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6785,13 +6828,13 @@
       <c r="AA25" s="43"/>
       <c r="AB25" s="27"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="23">
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6799,10 +6842,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -6823,13 +6866,13 @@
       <c r="AA26" s="43"/>
       <c r="AB26" s="27"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="23">
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -6840,7 +6883,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -6859,13 +6902,13 @@
       <c r="AA27" s="43"/>
       <c r="AB27" s="27"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="23">
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -6877,29 +6920,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -6909,13 +6952,13 @@
       <c r="AA28" s="43"/>
       <c r="AB28" s="27"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="23">
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -6937,21 +6980,21 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="23">
         <v>26</v>
@@ -6983,7 +7026,7 @@
       <c r="AA30" s="43"/>
       <c r="AB30" s="27"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="12"/>
       <c r="B31" s="23">
         <v>27</v>
@@ -7015,7 +7058,7 @@
       <c r="AA31" s="43"/>
       <c r="AB31" s="27"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
       <c r="B32" s="23">
         <v>28</v>
@@ -7047,7 +7090,7 @@
       <c r="AA32" s="26"/>
       <c r="AB32" s="27"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" s="12"/>
       <c r="B33" s="23">
         <v>29</v>
@@ -7079,13 +7122,13 @@
       <c r="AA33" s="26"/>
       <c r="AB33" s="27"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A34" s="12"/>
       <c r="B34" s="23">
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7093,7 +7136,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7109,7 +7152,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7117,13 +7160,13 @@
       <c r="AA34" s="26"/>
       <c r="AB34" s="27"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" s="12"/>
       <c r="B35" s="23">
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7132,7 +7175,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7153,13 +7196,13 @@
       <c r="AA35" s="26"/>
       <c r="AB35" s="27"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="23">
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7171,17 +7214,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7195,13 +7238,13 @@
       <c r="AA36" s="26"/>
       <c r="AB36" s="27"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="B37" s="23">
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7218,19 +7261,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7239,7 +7282,7 @@
       <c r="AA37" s="26"/>
       <c r="AB37" s="27"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" s="12"/>
       <c r="B38" s="23">
         <v>34</v>
@@ -7271,7 +7314,7 @@
       <c r="AA38" s="26"/>
       <c r="AB38" s="27"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" s="12"/>
       <c r="B39" s="23">
         <v>35</v>
@@ -7303,7 +7346,7 @@
       <c r="AA39" s="26"/>
       <c r="AB39" s="27"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" s="12"/>
       <c r="B40" s="23">
         <v>36</v>
@@ -7335,7 +7378,7 @@
       <c r="AA40" s="26"/>
       <c r="AB40" s="27"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
       <c r="B41" s="23">
         <v>37</v>
@@ -7367,7 +7410,7 @@
       <c r="AA41" s="26"/>
       <c r="AB41" s="27"/>
     </row>
-    <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="12"/>
       <c r="B42" s="28">
         <v>38</v>
@@ -7399,11 +7442,11 @@
       <c r="AA42" s="31"/>
       <c r="AB42" s="32"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7442,305 +7485,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-    </row>
-    <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>28</v>
-      </c>
-      <c r="B34" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7913,11 +7657,315 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E34"/>
+  <sheetViews>
+    <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
       <selection activeCell="D20" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
@@ -8008,7 +8056,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
@@ -8016,7 +8064,7 @@
         <v>216</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8025,15 +8073,15 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8083,7 +8131,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -8257,7 +8305,7 @@
         <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8277,7 +8325,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8297,7 +8345,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8357,9 +8405,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -8393,7 +8441,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -8462,7 +8510,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8481,7 +8529,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8500,7 +8548,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8516,7 +8564,7 @@
         <v>150</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8569,7 +8617,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -8755,10 +8803,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D20" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8766,7 +8814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>16</v>
       </c>
@@ -8960,7 +9008,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D20" t="s">
         <v>163</v>
@@ -9538,7 +9586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>34</v>
       </c>
@@ -9557,7 +9605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>36</v>
       </c>
@@ -9573,7 +9621,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>38</v>
       </c>
@@ -9589,7 +9637,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>40</v>
       </c>
@@ -9603,28 +9651,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="7"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B51" s="7"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B52" s="7"/>
     </row>
   </sheetData>
@@ -9975,7 +10023,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>40</v>
       </c>
@@ -9989,14 +10037,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -10363,17 +10411,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -10548,37 +10596,37 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>27</v>
       </c>
@@ -10665,7 +10713,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10699,12 +10747,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -10824,12 +10872,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -10933,7 +10981,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in SQ9 and in AutoStart2Kpumps.st. Updated documentation.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="399">
   <si>
     <t>Step #</t>
   </si>
@@ -1649,9 +1649,6 @@
     <t>Waiting for LT600 &lt; LT600 Min in Intermittent mode then goto 16 or changing to PID mode then goto 10 or stop Dewar or stop Seq9 and goto 22</t>
   </si>
   <si>
-    <t>Do you want to close the valve of the Dewar? Yes - goto 26; No - goto 18</t>
-  </si>
-  <si>
     <t>Waiting for CV590 to close or in state_stopping then goto 28</t>
   </si>
   <si>
@@ -1722,16 +1719,10 @@
     <t>In Intermittent mode goto 41, in Reg mode goto 32 or Stop and goto 0</t>
   </si>
   <si>
-    <t>Goto 7, if in intermittent mode set FV601 mem, Can be stopped</t>
-  </si>
-  <si>
     <t>Waiting for LT600 &lt; P_LT600_min then goto 42</t>
   </si>
   <si>
     <t>Wait for level to go below min.</t>
-  </si>
-  <si>
-    <t>Waiting for stop Seq9 or Stop Liquefier mode then goto 48 or and Waiting for LT600 &lt; LT600 Min in Intermittent mode and goto 42 or changing to PID mode and goto 34</t>
   </si>
   <si>
     <t>HNOSS comm OK and CV5203 status closed and CV5203 PercOut &lt;= 0 then goto 38</t>
@@ -2121,9 +2112,6 @@
     <t>Sequence 10: Cavity cooling (revised 2019-03-08)</t>
   </si>
   <si>
-    <t>State 36 - HNOSS valve has been closed by the PLC although CV5203 was in supervisory mode (not closed loop) - check why</t>
-  </si>
-  <si>
     <t>Add the reminder to close the LN2 valve when stopping the sequence</t>
   </si>
   <si>
@@ -2235,10 +2223,19 @@
     <t>Sequence 9: Valve Box cooling &amp; controlling level in 4K tank (Revised 2021-04-21)</t>
   </si>
   <si>
-    <t xml:space="preserve">Wait for TT602 or TT614 to go below TT Cool-down and CV5203 pERCoUT = 100 and HNOSS comm OK then goto 44. </t>
-  </si>
-  <si>
-    <t>Waiting for LT600 &gt; LT600 Max then goto 46 or ait for changing to PID mode and goto 34. Can be stopped.</t>
+    <t>Do you want to close the valve of the Dewar? Yes - goto 26; No - goto 28</t>
+  </si>
+  <si>
+    <t>Goto 7, if in intermittent mode set FV601 mem, When stopping goto 0</t>
+  </si>
+  <si>
+    <t>Wait for TT602 or TT614 to go below TT Cool-down and CV5203 pERCoUT = 100 and HNOSS comm OK then goto 44. When stopping goto 46</t>
+  </si>
+  <si>
+    <t>Waiting for LT600 &gt; LT600 Max then goto 46 or ait for changing to PID mode and goto 34. When stopping goto 46.</t>
+  </si>
+  <si>
+    <t>Waiting for stop Seq9 or Stop Liquefier mode then goto 48 or and Waiting for LT600 &lt; LT600 Min in Intermittent mode and goto 42 or changing to PID mode and goto 34. When stopping goto 48</t>
   </si>
 </sst>
 </file>
@@ -3579,7 +3576,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3588,27 +3585,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3693,7 +3690,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3713,8 +3710,8 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,7 +3724,7 @@
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="50" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -3981,7 +3978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>24</v>
       </c>
@@ -3992,7 +3989,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>233</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4008,7 +4005,7 @@
         <v>61</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4024,7 +4021,7 @@
         <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4040,7 +4037,7 @@
         <v>68</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4056,7 +4053,7 @@
         <v>63</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4072,7 +4069,7 @@
         <v>65</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4085,10 +4082,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
+        <v>237</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4099,7 +4096,7 @@
         <v>66</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4115,7 +4112,7 @@
         <v>62</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4123,7 +4120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>40</v>
       </c>
@@ -4131,7 +4128,7 @@
         <v>67</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>243</v>
+        <v>395</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4144,10 +4141,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4158,7 +4155,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4174,7 +4171,7 @@
         <v>69</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4182,7 +4179,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>46</v>
       </c>
@@ -4190,7 +4187,7 @@
         <v>70</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>246</v>
+        <v>398</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4206,27 +4203,25 @@
         <v>66</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B62" s="35" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B64" s="39" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="39"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4261,7 +4256,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="50" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C3" s="50"/>
       <c r="D3" s="50"/>
@@ -4327,7 +4322,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4340,7 +4335,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4356,7 +4351,7 @@
         <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4372,7 +4367,7 @@
         <v>79</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4388,7 +4383,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4401,10 +4396,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4412,7 +4407,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4423,7 +4418,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4439,7 +4434,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4455,22 +4450,22 @@
         <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -4636,12 +4631,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -4674,7 +4669,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -4740,7 +4735,7 @@
         <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4756,7 +4751,7 @@
         <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4764,10 +4759,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4778,7 +4773,7 @@
         <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4794,7 +4789,7 @@
         <v>59</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4815,7 +4810,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -4850,14 +4845,14 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="55" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C3" s="55"/>
       <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="53" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
@@ -4921,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5046,7 +5041,7 @@
         <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5063,7 +5058,7 @@
         <v>113</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5100,7 +5095,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5134,7 +5129,7 @@
         <v>119</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5142,19 +5137,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5164,37 +5159,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5230,7 +5225,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -5278,7 +5273,7 @@
         <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5294,7 +5289,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5302,10 +5297,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5316,7 +5311,7 @@
         <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5332,7 +5327,7 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5348,7 +5343,7 @@
         <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5364,12 +5359,12 @@
         <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5889,7 +5884,7 @@
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="49" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
@@ -5921,83 +5916,83 @@
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>319</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6038,16 +6033,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6078,14 +6073,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6114,7 +6109,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6122,7 +6117,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6150,7 +6145,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6159,7 +6154,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6186,7 +6181,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6197,47 +6192,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6248,7 +6243,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6259,7 +6254,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6284,7 +6279,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6296,7 +6291,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6320,7 +6315,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6333,7 +6328,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6356,7 +6351,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6370,7 +6365,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6392,7 +6387,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6407,7 +6402,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6428,7 +6423,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6444,7 +6439,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6464,7 +6459,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6481,7 +6476,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6500,7 +6495,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6518,7 +6513,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6536,7 +6531,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6555,10 +6550,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6574,7 +6569,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6594,7 +6589,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6610,7 +6605,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6632,7 +6627,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6646,7 +6641,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6668,7 +6663,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6682,7 +6677,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6705,7 +6700,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6718,7 +6713,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6742,13 +6737,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6758,7 +6753,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6782,13 +6777,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6798,14 +6793,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6834,7 +6829,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6842,10 +6837,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -6872,7 +6867,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -6883,7 +6878,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -6908,7 +6903,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -6920,29 +6915,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -6958,7 +6953,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -6980,16 +6975,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7128,7 +7123,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7136,7 +7131,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7152,7 +7147,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7166,7 +7161,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7175,7 +7170,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7202,7 +7197,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7214,17 +7209,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7244,7 +7239,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7261,19 +7256,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7446,7 +7441,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7675,7 +7670,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
@@ -7815,7 +7810,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8064,7 +8059,7 @@
         <v>216</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8078,10 +8073,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8131,7 +8126,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -8305,7 +8300,7 @@
         <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8325,7 +8320,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8345,7 +8340,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8407,7 +8402,7 @@
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -8441,7 +8436,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="50" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -8510,7 +8505,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8529,7 +8524,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8548,7 +8543,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8564,7 +8559,7 @@
         <v>150</v>
       </c>
       <c r="D16" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8617,7 +8612,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -8803,10 +8798,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D20" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -9008,7 +9003,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D20" t="s">
         <v>163</v>
@@ -9653,17 +9648,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10039,12 +10034,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -10411,17 +10406,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -10713,7 +10708,7 @@
         <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10747,12 +10742,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -10872,12 +10867,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -10981,7 +10976,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for SQ4 (HV tests). Not complete yet. Add sequence status bits to the sequence panels.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="407">
   <si>
     <t>Step #</t>
   </si>
@@ -993,16 +993,7 @@
     <t>Sequence 4: Magnet insert, HV tests</t>
   </si>
   <si>
-    <t>Transition to step 6</t>
-  </si>
-  <si>
-    <t>Sequence not ready, unconditional transition to stopping</t>
-  </si>
-  <si>
     <t>Stopping</t>
-  </si>
-  <si>
-    <t>Sequence not ready, unconditional transition to not running</t>
   </si>
   <si>
     <t>Sequence 5: Valve Box thermal shield cooling</t>
@@ -2236,6 +2227,39 @@
   </si>
   <si>
     <t>Waiting for stop Seq9 or Stop Liquefier mode then goto 48 or and Waiting for LT600 &lt; LT600 Min in Intermittent mode and goto 42 or changing to PID mode and goto 34. When stopping goto 48</t>
+  </si>
+  <si>
+    <t>Seq. 16 step 4 or Seq. 17 step 20 must be running</t>
+  </si>
+  <si>
+    <t>Waiting for Yes/No</t>
+  </si>
+  <si>
+    <t>Set relevant PVs in the Sim mode, turn off actuators for the valves and heaters. Operator disconnects the cable and confirms it by pressing Yes</t>
+  </si>
+  <si>
+    <t>Restoring connection to PVs</t>
+  </si>
+  <si>
+    <t>Gracefull transition to normal operation</t>
+  </si>
+  <si>
+    <t>Are the cables disconnected? - waiting for "Yes"</t>
+  </si>
+  <si>
+    <t>HV test (waiting for stop)</t>
+  </si>
+  <si>
+    <t>Control the flow/pressure. Waiting for "Stop" after reconnecting the cables</t>
+  </si>
+  <si>
+    <t>Wait for confirmation to start the tests.</t>
+  </si>
+  <si>
+    <t>Resets the Sim mode, rstores the proper control of the heaters and valves. Automatic transition to 12 after 5 s</t>
+  </si>
+  <si>
+    <t>When done exit the sequence</t>
   </si>
 </sst>
 </file>
@@ -2690,7 +2714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -2802,6 +2826,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2825,7 +2850,7 @@
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2849,6 +2874,12 @@
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3191,9 +3222,9 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Step #"/>
-    <tableColumn id="2" name="Name"/>
+    <tableColumn id="2" name="Name" dataDxfId="9"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note"/>
+    <tableColumn id="3" name="Note" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3568,7 +3599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3576,7 +3607,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3585,27 +3616,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -3633,7 +3664,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -3685,12 +3716,12 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3710,7 +3741,7 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -3723,21 +3754,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>393</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>390</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="B4" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3787,13 +3818,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3806,10 +3837,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3822,13 +3853,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3836,10 +3867,10 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3852,10 +3883,10 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3868,7 +3899,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3876,10 +3907,10 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3892,10 +3923,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3903,10 +3934,10 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3919,10 +3950,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3935,10 +3966,10 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3951,10 +3982,10 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3967,10 +3998,10 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3978,18 +4009,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4002,10 +4033,10 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4018,10 +4049,10 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4034,10 +4065,10 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4050,10 +4081,10 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4066,10 +4097,10 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4082,10 +4113,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4093,10 +4124,10 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4109,10 +4140,10 @@
         <v>38</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4120,15 +4151,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4141,21 +4172,21 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>42</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4163,15 +4194,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>44</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4179,15 +4210,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4200,28 +4231,28 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B62" s="35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B64" s="39"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4242,7 +4273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -4255,18 +4286,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>360</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>357</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="B4" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4316,13 +4347,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4335,7 +4366,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4348,10 +4379,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4364,10 +4395,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4380,10 +4411,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4396,10 +4427,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4407,7 +4438,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4415,10 +4446,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4431,10 +4462,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4447,25 +4478,25 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4500,11 +4531,11 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -4559,10 +4590,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4575,10 +4606,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4591,10 +4622,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4607,10 +4638,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4623,20 +4654,20 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -4668,21 +4699,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>260</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
+      <c r="A4" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4732,10 +4763,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4748,10 +4779,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4759,10 +4790,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4770,10 +4801,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4786,10 +4817,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4802,15 +4833,15 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -4844,19 +4875,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="53" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="54" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4910,13 +4941,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4930,13 +4961,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4950,10 +4981,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4967,10 +4998,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4984,13 +5015,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5004,10 +5035,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5021,10 +5052,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5038,10 +5069,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5055,10 +5086,10 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5072,10 +5103,10 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5089,13 +5120,13 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5109,10 +5140,10 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5126,10 +5157,10 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5137,19 +5168,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5159,37 +5190,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5224,19 +5255,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="B4" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5270,10 +5301,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5286,10 +5317,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5297,10 +5328,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5308,10 +5339,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5324,10 +5355,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5340,10 +5371,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5356,15 +5387,15 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -5398,20 +5429,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
+      <c r="A4" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5466,10 +5497,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5483,10 +5514,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5500,10 +5531,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5517,10 +5548,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -5554,20 +5585,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="50" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
+      <c r="B3" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5617,13 +5648,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5636,10 +5667,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5652,10 +5683,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5668,10 +5699,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5684,10 +5715,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5700,10 +5731,10 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -5738,18 +5769,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5799,10 +5830,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5815,10 +5846,10 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -5838,8 +5869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5883,116 +5914,116 @@
     </row>
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
-      <c r="B2" s="49" t="s">
-        <v>345</v>
-      </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
+      <c r="B2" s="50" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
     </row>
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>316</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>318</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6033,16 +6064,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6073,14 +6104,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6109,7 +6140,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6117,7 +6148,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6145,7 +6176,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6154,7 +6185,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6181,7 +6212,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6192,47 +6223,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6243,7 +6274,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6254,7 +6285,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6279,7 +6310,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6291,7 +6322,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6315,7 +6346,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6328,7 +6359,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6351,7 +6382,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6365,7 +6396,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6387,7 +6418,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6402,7 +6433,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6423,7 +6454,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6439,7 +6470,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6459,7 +6490,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6476,7 +6507,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6495,7 +6526,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6513,7 +6544,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6531,7 +6562,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6550,10 +6581,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6569,7 +6600,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6589,7 +6620,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6605,7 +6636,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6627,7 +6658,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6641,7 +6672,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6663,7 +6694,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6677,7 +6708,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6700,7 +6731,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6713,7 +6744,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6737,13 +6768,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6753,7 +6784,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6777,13 +6808,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6793,14 +6824,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6829,7 +6860,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6837,10 +6868,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -6867,7 +6898,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -6878,7 +6909,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -6903,7 +6934,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -6915,29 +6946,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -6953,7 +6984,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -6975,16 +7006,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -6994,11 +7025,15 @@
       <c r="B30" s="23">
         <v>26</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="44" t="s">
+        <v>396</v>
+      </c>
       <c r="D30" s="45"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="G30" s="43" t="s">
+        <v>318</v>
+      </c>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
       <c r="J30" s="43"/>
@@ -7123,7 +7158,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7131,7 +7166,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7147,7 +7182,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7161,7 +7196,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7170,7 +7205,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7197,7 +7232,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7209,17 +7244,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7239,7 +7274,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7256,19 +7291,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7405,7 +7440,7 @@
       <c r="AA41" s="26"/>
       <c r="AB41" s="27"/>
     </row>
-    <row r="42" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="28">
         <v>38</v>
@@ -7437,11 +7472,11 @@
       <c r="AA42" s="31"/>
       <c r="AB42" s="32"/>
     </row>
-    <row r="43" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7495,11 +7530,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7554,10 +7589,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7570,10 +7605,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7586,10 +7621,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7602,10 +7637,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7618,10 +7653,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7634,10 +7669,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -7670,15 +7705,15 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7734,13 +7769,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7753,13 +7788,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7772,10 +7807,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7788,10 +7823,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7804,13 +7839,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7823,10 +7858,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7839,10 +7874,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7855,10 +7890,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7871,10 +7906,10 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7887,10 +7922,10 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7903,13 +7938,13 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7922,10 +7957,10 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7938,10 +7973,10 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -7976,11 +8011,11 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="50" t="s">
-        <v>213</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -8039,10 +8074,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8056,10 +8091,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8073,10 +8108,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8090,10 +8125,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -8125,18 +8160,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>376</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8189,10 +8224,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8206,13 +8241,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8226,13 +8261,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8246,10 +8281,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8263,10 +8298,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8280,10 +8315,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8297,10 +8332,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8314,13 +8349,13 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8334,13 +8369,13 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8354,13 +8389,13 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8374,13 +8409,13 @@
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8394,15 +8429,15 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -8435,18 +8470,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>280</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8486,7 +8521,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8499,13 +8534,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8518,13 +8553,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8537,13 +8572,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8556,10 +8591,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8572,10 +8607,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8588,10 +8623,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8604,15 +8639,15 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -8645,18 +8680,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8696,7 +8731,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8709,13 +8744,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8728,13 +8763,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8747,13 +8782,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8766,10 +8801,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8782,10 +8817,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8798,10 +8833,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D20" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8814,10 +8849,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -8850,18 +8885,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8901,7 +8936,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8914,13 +8949,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8933,13 +8968,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8952,13 +8987,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -8971,10 +9006,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8987,10 +9022,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -9003,10 +9038,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D20" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -9039,18 +9074,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9090,7 +9125,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9103,10 +9138,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9119,10 +9154,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9138,7 +9173,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -9171,18 +9206,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9222,7 +9257,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9235,10 +9270,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9251,10 +9286,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9270,7 +9305,7 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -9648,17 +9683,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10034,12 +10069,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -10406,17 +10441,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -10434,7 +10469,7 @@
   <dimension ref="A3:D33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10466,165 +10501,260 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="49">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="49"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="49">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="C7" s="49"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="49">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="49">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="B9" s="5"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="49">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
+      <c r="B10" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C10" s="49">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="49">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="B11" s="5"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="49">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
+      <c r="B12" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" s="49">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="49">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="B13" s="5"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="49">
         <v>8</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="49">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="49">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="B15" s="5"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="B16" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C16" s="49"/>
+      <c r="D16" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="49">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="B17" s="5"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="49">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="B18" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C18" s="49"/>
+      <c r="D18" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="49">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="B19" s="5"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20" s="49">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="B20" s="5"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A21" s="49">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="B21" s="5"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A22" s="49">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="B22" s="5"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A23" s="49">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="B23" s="5"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A24" s="49">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A25" s="49">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A26">
+      <c r="B25" s="5"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A26" s="49">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A27">
+      <c r="B26" s="5"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A27" s="49">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A28">
+      <c r="B27" s="5"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A28" s="49">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A29">
+      <c r="B28" s="5"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A29" s="49">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A30">
+      <c r="B29" s="5"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A30" s="49">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A31">
+      <c r="B30" s="5"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A31" s="49">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A32">
+      <c r="B31" s="5"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A32" s="49">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A33">
+      <c r="B32" s="5"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A33" s="49">
         <v>27</v>
       </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10653,7 +10783,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -10705,10 +10835,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10721,7 +10851,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10734,20 +10864,20 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -10778,7 +10908,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -10830,10 +10960,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10846,7 +10976,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10859,20 +10989,20 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -10903,7 +11033,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -10955,10 +11085,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10971,12 +11101,12 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the PLC program to deal with magnet quench at 2K.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="415">
   <si>
     <t>Step #</t>
   </si>
@@ -1477,9 +1477,6 @@
   </si>
   <si>
     <t>Warning flow SQ15_PT660 not available in epics. Maybe we should create such a bit in EPICS DB. PT660 Max is used for the limit. There are more warnings in this sequence: FIC583_conditions (dT/dL and dT/dt above max limits),  LIC682_conditions (FT583 and PT681 below limits), LIC683_conditions (FT581 &lt; SP FT581 and PT660 &lt; SP PT660)</t>
-  </si>
-  <si>
-    <t>Sequence 16: Magnet, 4K operation</t>
   </si>
   <si>
     <t>Waiting for State_Stopping then goto 6</t>
@@ -2260,6 +2257,46 @@
   </si>
   <si>
     <t>When done exit the sequence</t>
+  </si>
+  <si>
+    <t>Sequence 16: Magnet, 4K operation (Added quench detection logic, 2021-09-30)</t>
+  </si>
+  <si>
+    <t>Quench detected</t>
+  </si>
+  <si>
+    <t>Filling from below</t>
+  </si>
+  <si>
+    <t>Filling from above</t>
+  </si>
+  <si>
+    <t>Wait until LI680 &gt; commisioning parameter threshold then goto 4</t>
+  </si>
+  <si>
+    <t>to be decided then goto 4</t>
+  </si>
+  <si>
+    <t>Recovering from quench</t>
+  </si>
+  <si>
+    <t>Closing the Lhe supply, waiting for PT681 to go below SP_PIC681 then goto 10</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Start to regulate PT681, open FV587 then goto 12 or 14 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Before the test just wait for operators answer to continue</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2714,7 +2751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -2827,6 +2864,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2845,12 +2890,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2920,7 +2971,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="6"/>
+    <tableColumn id="3" name="Note" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2936,7 +2987,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="5"/>
+    <tableColumn id="3" name="Note" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2968,7 +3019,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="4"/>
+    <tableColumn id="3" name="Note" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3000,7 +3051,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="3"/>
+    <tableColumn id="3" name="Note" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3023,8 +3074,8 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1345678910111218" displayName="Table1345678910111218" ref="A4:D11" totalsRowShown="0">
-  <autoFilter ref="A4:D11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table1345678910111218" displayName="Table1345678910111218" ref="A4:D19" totalsRowShown="0">
+  <autoFilter ref="A4:D19"/>
   <sortState ref="A5:C45">
     <sortCondition ref="A4:A45"/>
   </sortState>
@@ -3032,7 +3083,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note"/>
+    <tableColumn id="3" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3048,7 +3099,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="2"/>
+    <tableColumn id="3" name="Note" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3064,7 +3115,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="1"/>
+    <tableColumn id="3" name="Note" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3096,7 +3147,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="0"/>
+    <tableColumn id="3" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3222,9 +3273,9 @@
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Step #"/>
-    <tableColumn id="2" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" name="Name" dataDxfId="10"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="8"/>
+    <tableColumn id="3" name="Note" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3304,7 +3355,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="7"/>
+    <tableColumn id="3" name="Note" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3599,7 +3650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3607,7 +3658,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3616,27 +3667,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3721,7 +3772,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3741,7 +3792,7 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -3754,21 +3805,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="51" t="s">
-        <v>390</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3840,7 +3891,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3853,13 +3904,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3870,7 +3921,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3886,7 +3937,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3899,7 +3950,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3910,7 +3961,7 @@
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3923,10 +3974,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3937,7 +3988,7 @@
         <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3953,7 +4004,7 @@
         <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3969,7 +4020,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3985,7 +4036,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4001,7 +4052,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4020,7 +4071,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4036,7 +4087,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4052,7 +4103,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4068,7 +4119,7 @@
         <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4084,7 +4135,7 @@
         <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4100,7 +4151,7 @@
         <v>62</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4113,10 +4164,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
+        <v>233</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4127,7 +4178,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4143,7 +4194,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4159,7 +4210,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4172,10 +4223,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4186,7 +4237,7 @@
         <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4202,7 +4253,7 @@
         <v>66</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4218,7 +4269,7 @@
         <v>67</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4234,17 +4285,17 @@
         <v>63</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B61" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B62" s="35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4252,7 +4303,7 @@
     </row>
     <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B66" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -4286,18 +4337,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="51" t="s">
-        <v>357</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>356</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4353,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4366,7 +4417,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4382,7 +4433,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4398,7 +4449,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4414,7 +4465,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4427,10 +4478,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4438,7 +4489,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4449,7 +4500,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4465,7 +4516,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4481,22 +4532,22 @@
         <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -4531,11 +4582,11 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -4662,12 +4713,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -4699,21 +4750,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
-        <v>257</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="A3" s="55" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4766,7 +4817,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4782,7 +4833,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4790,10 +4841,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" t="s">
         <v>253</v>
-      </c>
-      <c r="D13" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4804,7 +4855,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4820,7 +4871,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4841,7 +4892,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -4875,19 +4926,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="56" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="B3" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="54" t="s">
-        <v>262</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4947,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5072,7 +5123,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5089,7 +5140,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5126,7 +5177,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5160,7 +5211,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5168,19 +5219,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5190,37 +5241,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B44" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B45" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5255,19 +5306,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="A3" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5304,7 +5355,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5320,7 +5371,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5328,10 +5379,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5342,7 +5393,7 @@
         <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5358,7 +5409,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5374,7 +5425,7 @@
         <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5390,12 +5441,12 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -5429,20 +5480,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5585,20 +5636,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5753,110 +5804,173 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="53" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="53">
+        <v>0</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="53">
+        <v>1</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="53">
+        <v>2</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="53">
+        <v>4</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-    </row>
-    <row r="3" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="53">
+        <v>6</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="53">
+        <v>8</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>407</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="53">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="53">
+        <v>10</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="53">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>189</v>
-      </c>
-      <c r="D11" t="s">
-        <v>190</v>
+      <c r="D15" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="53">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="53">
+        <v>12</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>408</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="53">
+        <v>14</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>409</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:E3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
@@ -5869,7 +5983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -5914,116 +6028,116 @@
     </row>
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
-      <c r="B2" s="50" t="s">
-        <v>342</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
+      <c r="B2" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
     </row>
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>315</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6064,16 +6178,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>318</v>
-      </c>
       <c r="E5" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6104,14 +6218,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6140,7 +6254,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6148,7 +6262,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6176,7 +6290,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6185,7 +6299,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6212,7 +6326,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6223,47 +6337,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6274,7 +6388,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6285,7 +6399,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6310,7 +6424,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6322,7 +6436,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6346,7 +6460,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6359,7 +6473,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6382,7 +6496,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6396,7 +6510,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6418,7 +6532,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6433,7 +6547,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6454,7 +6568,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6470,7 +6584,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6490,7 +6604,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6507,7 +6621,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6526,7 +6640,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6544,7 +6658,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6562,7 +6676,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6581,10 +6695,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6600,7 +6714,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6620,7 +6734,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6636,7 +6750,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6658,7 +6772,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6672,7 +6786,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6694,7 +6808,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6708,7 +6822,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6731,7 +6845,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6744,7 +6858,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6768,13 +6882,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6784,7 +6898,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6808,13 +6922,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6824,14 +6938,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6860,7 +6974,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6868,10 +6982,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -6898,7 +7012,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -6909,7 +7023,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -6934,7 +7048,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -6946,29 +7060,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -6984,7 +7098,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -7006,16 +7120,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7026,13 +7140,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
@@ -7158,7 +7272,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7166,7 +7280,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7182,7 +7296,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7196,7 +7310,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7205,7 +7319,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7232,7 +7346,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7244,17 +7358,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7274,7 +7388,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7291,19 +7405,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7476,7 +7590,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7530,11 +7644,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="51" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7589,10 +7703,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7605,10 +7719,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7624,7 +7738,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7637,10 +7751,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7653,10 +7767,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7669,10 +7783,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -7705,15 +7819,15 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="51" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7775,7 +7889,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7845,7 +7959,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7877,7 +7991,7 @@
         <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7893,7 +8007,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7925,7 +8039,7 @@
         <v>112</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7944,7 +8058,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7976,7 +8090,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -8011,11 +8125,11 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -8074,10 +8188,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8091,10 +8205,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8108,10 +8222,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
+        <v>385</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>386</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8125,10 +8239,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -8160,18 +8274,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
-        <v>373</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="A3" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8335,7 +8449,7 @@
         <v>140</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8355,7 +8469,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8375,7 +8489,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8437,7 +8551,7 @@
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -8470,18 +8584,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
-        <v>277</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="A3" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8540,7 +8654,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8559,7 +8673,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8578,7 +8692,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8594,7 +8708,7 @@
         <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8647,7 +8761,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -8680,18 +8794,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8804,7 +8918,7 @@
         <v>158</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8833,10 +8947,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8885,18 +8999,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8974,7 +9088,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9038,7 +9152,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D20" t="s">
         <v>160</v>
@@ -9074,18 +9188,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9206,18 +9320,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9683,17 +9797,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10069,12 +10183,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -10091,7 +10205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -10441,17 +10555,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -10543,13 +10657,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C10" s="49">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10565,13 +10679,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C12" s="49">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10587,13 +10701,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C14" s="49">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10609,11 +10723,11 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10629,11 +10743,11 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10838,7 +10952,7 @@
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10872,12 +10986,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -10997,12 +11111,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -11106,7 +11220,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SQ16 modified to deal with magnet's quench.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" firstSheet="1" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -2259,9 +2259,6 @@
     <t>When done exit the sequence</t>
   </si>
   <si>
-    <t>Sequence 16: Magnet, 4K operation (Added quench detection logic, 2021-09-30)</t>
-  </si>
-  <si>
     <t>Quench detected</t>
   </si>
   <si>
@@ -2295,8 +2292,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Before the test just wait for operators answer to continue</t>
+      <t>Before the test just wait for operators answer to continue and goto 4</t>
     </r>
+  </si>
+  <si>
+    <t>Sequence 16: Magnet, 4K operation (Added quench detection logic, 2021-10-01)</t>
   </si>
 </sst>
 </file>
@@ -5807,7 +5807,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5821,7 +5821,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -5913,10 +5913,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5929,13 +5929,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C15" s="53">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5948,10 +5948,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5964,10 +5964,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some bugs in SQ15. Updated documentation. Updated opi.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" firstSheet="1" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="419">
   <si>
     <t>Step #</t>
   </si>
@@ -1452,16 +1452,10 @@
     <t>Waiting for PT600 &gt; Max Pressure then goto 8. Possible to uncheck the Isolated (goes to 4) or stop the seq.</t>
   </si>
   <si>
-    <t>Sequence 15: Magnet cooling down</t>
-  </si>
-  <si>
     <t>Have you chosen the recovery circuit for the cryostat? Waiting for Yes then goto 6</t>
   </si>
   <si>
     <t>Cooling HX680 &amp; HX683</t>
-  </si>
-  <si>
-    <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8</t>
   </si>
   <si>
     <t>Finished cooling</t>
@@ -2297,6 +2291,24 @@
   </si>
   <si>
     <t>Sequence 16: Magnet, 4K operation (Added quench detection logic, 2021-10-01)</t>
+  </si>
+  <si>
+    <t>Sequence 15: Magnet cooling down (modified the PLC program on 2021-12-09)</t>
+  </si>
+  <si>
+    <t>Delaying</t>
+  </si>
+  <si>
+    <t>Delaying transition between state 6 and 7 for 3 min.</t>
+  </si>
+  <si>
+    <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8 or If TT608 &lt; 5K and TT664 &gt; 80 then goto 5</t>
+  </si>
+  <si>
+    <t>Cooling magnet with mixed Ghe</t>
+  </si>
+  <si>
+    <t>Do this until TT608 &gt; 5K or TT665 &lt;= 80 K then goto 6</t>
   </si>
 </sst>
 </file>
@@ -2872,6 +2884,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2890,9 +2905,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3083,7 +3095,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="0"/>
+    <tableColumn id="3" name="Note" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3099,7 +3111,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="3"/>
+    <tableColumn id="3" name="Note" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3115,7 +3127,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="2"/>
+    <tableColumn id="3" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3147,7 +3159,7 @@
     <tableColumn id="1" name="Step #"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="1"/>
+    <tableColumn id="3" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3658,7 +3670,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3667,27 +3679,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3772,7 +3784,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3805,21 +3817,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>387</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -3891,7 +3903,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3904,13 +3916,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3921,7 +3933,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3937,7 +3949,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3950,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3961,7 +3973,7 @@
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3974,10 +3986,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3988,7 +4000,7 @@
         <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4004,7 +4016,7 @@
         <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4020,7 +4032,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4036,7 +4048,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4052,7 +4064,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4071,7 +4083,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4087,7 +4099,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4103,7 +4115,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4119,7 +4131,7 @@
         <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4135,7 +4147,7 @@
         <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4151,7 +4163,7 @@
         <v>62</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4164,10 +4176,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4178,7 +4190,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4194,7 +4206,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4210,7 +4222,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4218,18 +4230,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>42</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4245,7 +4257,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>44</v>
       </c>
@@ -4253,7 +4265,7 @@
         <v>66</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4261,7 +4273,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>46</v>
       </c>
@@ -4269,7 +4281,7 @@
         <v>67</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4277,7 +4289,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>48</v>
       </c>
@@ -4285,25 +4297,25 @@
         <v>63</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="35" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="39"/>
     </row>
-    <row r="66" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -4337,18 +4349,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>356</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4404,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4417,7 +4429,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4433,7 +4445,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4449,7 +4461,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4465,7 +4477,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4478,10 +4490,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4489,7 +4501,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4500,7 +4512,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4516,7 +4528,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4532,22 +4544,22 @@
         <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4582,11 +4594,11 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -4713,12 +4725,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4750,21 +4762,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4817,7 +4829,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4833,7 +4845,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4841,10 +4853,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4855,7 +4867,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4871,7 +4883,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4892,7 +4904,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4926,19 +4938,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
+      <c r="B3" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="58" t="s">
-        <v>261</v>
-      </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="59" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -4998,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5123,7 +5135,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5140,7 +5152,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5177,7 +5189,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5211,7 +5223,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5219,19 +5231,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5241,37 +5253,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
+        <v>344</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B44" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B45" s="11" t="s">
-        <v>348</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5306,19 +5318,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -5355,7 +5367,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5371,7 +5383,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5379,10 +5391,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5393,7 +5405,7 @@
         <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5409,7 +5421,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5425,7 +5437,7 @@
         <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5441,12 +5453,12 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -5480,20 +5492,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5622,8 +5634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5636,20 +5648,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="55" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="A2" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:5" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="57" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="B3" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -5705,28 +5717,40 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>414</v>
+      </c>
+      <c r="D10" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>417</v>
+      </c>
+      <c r="D12" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5737,7 +5761,7 @@
         <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -5750,7 +5774,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D15" t="s">
         <v>135</v>
@@ -5769,7 +5793,7 @@
         <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5785,7 +5809,7 @@
         <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -5806,7 +5830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5821,11 +5845,11 @@
   <sheetData>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
-      <c r="D2" s="62"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="52"/>
@@ -5884,7 +5908,7 @@
         <v>85</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5897,10 +5921,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -5913,10 +5937,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5929,13 +5953,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C15" s="53">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5948,10 +5972,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>405</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5964,10 +5988,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="53" t="s">
+        <v>406</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -6028,116 +6052,116 @@
     </row>
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
-      <c r="B2" s="54" t="s">
-        <v>341</v>
-      </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="B2" s="55" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
     </row>
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>314</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6178,16 +6202,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6218,14 +6242,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6254,7 +6278,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6262,7 +6286,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6290,7 +6314,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6299,7 +6323,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6326,7 +6350,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6337,47 +6361,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6388,7 +6412,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6399,7 +6423,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6424,7 +6448,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6436,7 +6460,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6460,7 +6484,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6473,7 +6497,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6496,7 +6520,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6510,7 +6534,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6532,7 +6556,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6547,7 +6571,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6568,7 +6592,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6584,7 +6608,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6604,7 +6628,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6621,7 +6645,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6640,7 +6664,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6658,7 +6682,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6676,7 +6700,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6695,10 +6719,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6714,7 +6738,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6734,7 +6758,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6750,7 +6774,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6772,7 +6796,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6786,7 +6810,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6808,7 +6832,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6822,7 +6846,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6845,7 +6869,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6858,7 +6882,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6882,13 +6906,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6898,7 +6922,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6922,13 +6946,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6938,14 +6962,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6974,7 +6998,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6982,10 +7006,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -7012,7 +7036,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -7023,7 +7047,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -7048,7 +7072,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -7060,29 +7084,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -7098,7 +7122,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -7120,16 +7144,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7140,13 +7164,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
@@ -7272,7 +7296,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7280,7 +7304,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7296,7 +7320,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7310,7 +7334,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7319,7 +7343,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7346,7 +7370,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7358,17 +7382,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7388,7 +7412,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7405,19 +7429,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7590,7 +7614,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7644,11 +7668,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7703,10 +7727,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7719,10 +7743,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7738,7 +7762,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7751,10 +7775,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7767,10 +7791,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -7783,10 +7807,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -7819,15 +7843,15 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -7889,7 +7913,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7959,7 +7983,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -7991,7 +8015,7 @@
         <v>107</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8007,7 +8031,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8039,7 +8063,7 @@
         <v>112</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8047,7 +8071,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -8058,7 +8082,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8090,7 +8114,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -8125,11 +8149,11 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="55" t="s">
-        <v>209</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
@@ -8188,10 +8212,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8205,10 +8229,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8222,10 +8246,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8239,10 +8263,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -8274,18 +8298,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
-        <v>372</v>
-      </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="56" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8449,7 +8473,7 @@
         <v>140</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8469,7 +8493,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8489,7 +8513,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8551,7 +8575,7 @@
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -8584,18 +8608,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8654,7 +8678,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8673,7 +8697,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8692,7 +8716,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8708,7 +8732,7 @@
         <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8761,7 +8785,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -8794,18 +8818,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -8918,7 +8942,7 @@
         <v>158</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8947,10 +8971,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D20" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8999,18 +9023,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9088,7 +9112,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9152,7 +9176,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
         <v>160</v>
@@ -9188,18 +9212,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9320,18 +9344,18 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -9797,17 +9821,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10183,12 +10207,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -10555,17 +10579,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -10657,13 +10681,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C10" s="49">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10679,13 +10703,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C12" s="49">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10701,13 +10725,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C14" s="49">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10723,11 +10747,11 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10743,11 +10767,11 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10952,7 +10976,7 @@
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10986,12 +11010,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -11111,12 +11135,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -11220,7 +11244,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New magnet cooling algorithm: alternatively cool and warm GHe.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="417">
   <si>
     <t>Step #</t>
   </si>
@@ -2293,22 +2293,16 @@
     <t>Sequence 16: Magnet, 4K operation (Added quench detection logic, 2021-10-01)</t>
   </si>
   <si>
-    <t>Sequence 15: Magnet cooling down (modified the PLC program on 2021-12-09)</t>
-  </si>
-  <si>
-    <t>Delaying</t>
-  </si>
-  <si>
-    <t>Delaying transition between state 6 and 7 for 3 min.</t>
-  </si>
-  <si>
-    <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8 or If TT608 &lt; 5K and TT664 &gt; 80 then goto 5</t>
-  </si>
-  <si>
     <t>Cooling magnet with mixed Ghe</t>
   </si>
   <si>
-    <t>Do this until TT608 &gt; 5K or TT665 &lt;= 80 K then goto 6</t>
+    <t>Sequence 15: Magnet cooling down (modified the PLC program on 2021-12-23)</t>
+  </si>
+  <si>
+    <t>Stay in 7  until dT/dL is 2K below max value AND TT665 &gt; 80 K then goto 6, if stop goto 14</t>
+  </si>
+  <si>
+    <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8 OR If (dT/dL is too high (or other condition resetting "SQ15_FIC583_conditions") OR TT698 &lt; 5K) AND and TT665 &gt; 80  then goto 7 OR stop and then goto 14</t>
   </si>
 </sst>
 </file>
@@ -5635,7 +5629,7 @@
   <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5649,7 +5643,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="56" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -5720,18 +5714,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>414</v>
-      </c>
-      <c r="D10" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5742,18 +5725,18 @@
         <v>416</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>417</v>
-      </c>
-      <c r="D12" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+        <v>413</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Modified SQ18: after quench detection the program can go to the next step after pressing "Yes" button. Added sending the status of SQ4 to maglpc PLC.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="SQ14" sheetId="16" r:id="rId17"/>
     <sheet name="SQ15" sheetId="18" r:id="rId18"/>
     <sheet name="SQ16" sheetId="19" r:id="rId19"/>
-    <sheet name="SQ18" sheetId="21" r:id="rId20"/>
-    <sheet name="SQ17" sheetId="20" r:id="rId21"/>
+    <sheet name="SQ17" sheetId="20" r:id="rId20"/>
+    <sheet name="SQ18" sheetId="21" r:id="rId21"/>
     <sheet name="SQ19" sheetId="22" r:id="rId22"/>
     <sheet name="SQ20" sheetId="23" r:id="rId23"/>
     <sheet name="SQ21" sheetId="24" r:id="rId24"/>
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="418">
   <si>
     <t>Step #</t>
   </si>
@@ -1535,9 +1535,6 @@
     </r>
   </si>
   <si>
-    <t>Sequence 18: Magnet 2K operation - control of the level and the pressure</t>
-  </si>
-  <si>
     <t>Regulation two baths</t>
   </si>
   <si>
@@ -1548,9 +1545,6 @@
   </si>
   <si>
     <t>If quench detected - goto8 or if stopping seq 18 or 18 then goto 12</t>
-  </si>
-  <si>
-    <t>Wait until Normal_State.Ls_c and if LI680 &gt; P_LI680_max goto 10 else if LI680 &lt; P_LI680_max goto 14</t>
   </si>
   <si>
     <t>Wait until LT682 &gt; P_LT682 then goto 6</t>
@@ -2303,6 +2297,15 @@
   </si>
   <si>
     <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8 OR If (dT/dL is too high (or other condition resetting "SQ15_FIC583_conditions") OR TT698 &lt; 5K) AND and TT665 &gt; 80  then goto 7 OR stop and then goto 14</t>
+  </si>
+  <si>
+    <t>End of filling (quench detected)</t>
+  </si>
+  <si>
+    <t>Wait until (Normal_State.Ls_c or Yes answer) and if LI680 &gt; P_LI680_max goto 10 else if LI680 &lt; P_LI680_max goto 14</t>
+  </si>
+  <si>
+    <t>Sequence 18: Magnet 2K operation - control of the level and the pressure (2022-04-26 - added checcking "Yes" command when waiting for transition from step 8)</t>
   </si>
 </sst>
 </file>
@@ -2757,7 +2760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -2899,6 +2902,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3096,6 +3102,22 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
+  <autoFilter ref="A5:D34"/>
+  <sortState ref="A6:C46">
+    <sortCondition ref="A4:A45"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Step #"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="4" name="Message #"/>
+    <tableColumn id="3" name="Note" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table13456789101112141520" displayName="Table13456789101112141520" ref="A5:D20" totalsRowShown="0">
   <autoFilter ref="A5:D20"/>
   <sortState ref="A6:C46">
@@ -3106,22 +3128,6 @@
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
     <tableColumn id="3" name="Note" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
-  <autoFilter ref="A5:D34"/>
-  <sortState ref="A6:C46">
-    <sortCondition ref="A4:A45"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Step #"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3664,7 +3670,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3673,27 +3679,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3778,7 +3784,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3798,7 +3804,7 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -3812,7 +3818,7 @@
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -3897,7 +3903,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3910,13 +3916,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3927,7 +3933,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3943,7 +3949,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3956,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3967,7 +3973,7 @@
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3980,10 +3986,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3994,7 +4000,7 @@
         <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4010,7 +4016,7 @@
         <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4026,7 +4032,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4042,7 +4048,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4058,7 +4064,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4077,7 +4083,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4093,7 +4099,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4109,7 +4115,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4125,7 +4131,7 @@
         <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4141,7 +4147,7 @@
         <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4157,7 +4163,7 @@
         <v>62</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4170,10 +4176,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4184,7 +4190,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4200,7 +4206,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4216,7 +4222,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4229,10 +4235,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4243,7 +4249,7 @@
         <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4259,7 +4265,7 @@
         <v>66</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4275,7 +4281,7 @@
         <v>67</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4291,17 +4297,17 @@
         <v>63</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,7 +4315,7 @@
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4350,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -4410,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4423,7 +4429,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4439,7 +4445,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4455,7 +4461,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4471,7 +4477,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4484,10 +4490,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4495,7 +4501,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4506,7 +4512,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4522,7 +4528,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4538,22 +4544,22 @@
         <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4719,12 +4725,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4757,7 +4763,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -4823,7 +4829,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4839,7 +4845,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4847,10 +4853,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4861,7 +4867,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4877,7 +4883,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4898,7 +4904,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4933,14 +4939,14 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="61" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="59" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
@@ -5004,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5129,7 +5135,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5146,7 +5152,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5183,7 +5189,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5217,7 +5223,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5225,19 +5231,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5247,37 +5253,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5313,7 +5319,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -5361,7 +5367,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5377,7 +5383,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5385,10 +5391,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5399,7 +5405,7 @@
         <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5415,7 +5421,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5431,7 +5437,7 @@
         <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5447,12 +5453,12 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -5628,7 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -5643,7 +5649,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="56" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -5722,7 +5728,7 @@
         <v>179</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5730,10 +5736,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>411</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5828,7 +5834,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -5920,10 +5926,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5936,13 +5942,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C15" s="53">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5955,10 +5961,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>403</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>405</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5971,10 +5977,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -5990,7 +5996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -6036,7 +6042,7 @@
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="55" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="55"/>
@@ -6068,83 +6074,83 @@
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>311</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6185,16 +6191,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6225,14 +6231,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6261,7 +6267,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6269,7 +6275,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6297,7 +6303,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6306,7 +6312,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6333,7 +6339,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6344,47 +6350,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6395,7 +6401,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6406,7 +6412,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6431,7 +6437,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6443,7 +6449,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6467,7 +6473,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6480,7 +6486,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6503,7 +6509,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6517,7 +6523,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6539,7 +6545,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6554,7 +6560,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6575,7 +6581,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6591,7 +6597,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6611,7 +6617,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6628,7 +6634,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6647,7 +6653,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6665,7 +6671,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6683,7 +6689,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6702,10 +6708,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6721,7 +6727,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6741,7 +6747,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6757,7 +6763,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6779,7 +6785,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6793,7 +6799,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6815,7 +6821,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6829,7 +6835,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6852,7 +6858,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6865,7 +6871,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6889,13 +6895,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6905,7 +6911,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6929,13 +6935,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6945,14 +6951,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6981,7 +6987,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6989,10 +6995,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -7019,7 +7025,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -7030,7 +7036,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -7055,7 +7061,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -7067,29 +7073,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -7105,7 +7111,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -7127,16 +7133,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7147,13 +7153,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
@@ -7279,7 +7285,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7287,7 +7293,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7303,7 +7309,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7317,7 +7323,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7326,7 +7332,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7353,7 +7359,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7365,17 +7371,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7395,7 +7401,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7412,19 +7418,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7597,7 +7603,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7636,180 +7642,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="56" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-    </row>
-    <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>205</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
@@ -7826,7 +7658,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
@@ -7966,7 +7798,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8103,6 +7935,188 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8116,7 +8130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
@@ -8133,7 +8147,7 @@
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -8195,10 +8209,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8212,10 +8226,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8229,10 +8243,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8246,10 +8260,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -8282,7 +8296,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -8456,7 +8470,7 @@
         <v>140</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8476,7 +8490,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8496,7 +8510,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8558,7 +8572,7 @@
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -8592,7 +8606,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -8661,7 +8675,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8680,7 +8694,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8699,7 +8713,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8715,7 +8729,7 @@
         <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8768,7 +8782,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -8925,7 +8939,7 @@
         <v>158</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8954,10 +8968,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -9095,7 +9109,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9159,7 +9173,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D20" t="s">
         <v>160</v>
@@ -9804,17 +9818,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10190,12 +10204,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -10562,17 +10576,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -10664,13 +10678,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C10" s="49">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10686,13 +10700,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C12" s="49">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10708,13 +10722,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C14" s="49">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10730,11 +10744,11 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10750,11 +10764,11 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10959,7 +10973,7 @@
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10993,12 +11007,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -11118,12 +11132,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -11227,7 +11241,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified SQ18: after quench detection the program can go to the next step after pressing "Yes" button.
</commit_message>
<xml_diff>
--- a/doc/Sequences-steps.xlsx
+++ b/doc/Sequences-steps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24645" windowHeight="12105" firstSheet="10" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="29" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="SQ14" sheetId="16" r:id="rId17"/>
     <sheet name="SQ15" sheetId="18" r:id="rId18"/>
     <sheet name="SQ16" sheetId="19" r:id="rId19"/>
-    <sheet name="SQ18" sheetId="21" r:id="rId20"/>
-    <sheet name="SQ17" sheetId="20" r:id="rId21"/>
+    <sheet name="SQ17" sheetId="20" r:id="rId20"/>
+    <sheet name="SQ18" sheetId="21" r:id="rId21"/>
     <sheet name="SQ19" sheetId="22" r:id="rId22"/>
     <sheet name="SQ20" sheetId="23" r:id="rId23"/>
     <sheet name="SQ21" sheetId="24" r:id="rId24"/>
@@ -880,7 +880,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="418">
   <si>
     <t>Step #</t>
   </si>
@@ -1535,9 +1535,6 @@
     </r>
   </si>
   <si>
-    <t>Sequence 18: Magnet 2K operation - control of the level and the pressure</t>
-  </si>
-  <si>
     <t>Regulation two baths</t>
   </si>
   <si>
@@ -1548,9 +1545,6 @@
   </si>
   <si>
     <t>If quench detected - goto8 or if stopping seq 18 or 18 then goto 12</t>
-  </si>
-  <si>
-    <t>Wait until Normal_State.Ls_c and if LI680 &gt; P_LI680_max goto 10 else if LI680 &lt; P_LI680_max goto 14</t>
   </si>
   <si>
     <t>Wait until LT682 &gt; P_LT682 then goto 6</t>
@@ -2303,6 +2297,15 @@
   </si>
   <si>
     <t>Wait until TT680 &lt; SP_TT680 or LT683 &gt; SP_LT683 then goto 8 OR If (dT/dL is too high (or other condition resetting "SQ15_FIC583_conditions") OR TT698 &lt; 5K) AND and TT665 &gt; 80  then goto 7 OR stop and then goto 14</t>
+  </si>
+  <si>
+    <t>End of filling (quench detected)</t>
+  </si>
+  <si>
+    <t>Wait until (Normal_State.Ls_c or Yes answer) and if LI680 &gt; P_LI680_max goto 10 else if LI680 &lt; P_LI680_max goto 14</t>
+  </si>
+  <si>
+    <t>Sequence 18: Magnet 2K operation - control of the level and the pressure (2022-04-26 - added checcking "Yes" command when waiting for transition from step 8)</t>
   </si>
 </sst>
 </file>
@@ -2757,7 +2760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -2899,6 +2902,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3096,6 +3102,22 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
+  <autoFilter ref="A5:D34"/>
+  <sortState ref="A6:C46">
+    <sortCondition ref="A4:A45"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Step #"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="4" name="Message #"/>
+    <tableColumn id="3" name="Note" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table13456789101112141520" displayName="Table13456789101112141520" ref="A5:D20" totalsRowShown="0">
   <autoFilter ref="A5:D20"/>
   <sortState ref="A6:C46">
@@ -3106,22 +3128,6 @@
     <tableColumn id="2" name="Name"/>
     <tableColumn id="4" name="Message #"/>
     <tableColumn id="3" name="Note" dataDxfId="2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table134567891011121419" displayName="Table134567891011121419" ref="A5:D34" totalsRowShown="0">
-  <autoFilter ref="A5:D34"/>
-  <sortState ref="A6:C46">
-    <sortCondition ref="A4:A45"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Step #"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="4" name="Message #"/>
-    <tableColumn id="3" name="Note" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3664,7 +3670,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -3673,27 +3679,27 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="35" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3778,7 +3784,7 @@
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B12" s="35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3798,7 +3804,7 @@
   </sheetPr>
   <dimension ref="A3:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
@@ -3812,7 +3818,7 @@
   <sheetData>
     <row r="3" spans="1:7" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -3897,7 +3903,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3910,13 +3916,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -3927,7 +3933,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3943,7 +3949,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3956,7 +3962,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3967,7 +3973,7 @@
         <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -3980,10 +3986,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -3994,7 +4000,7 @@
         <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4010,7 +4016,7 @@
         <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4026,7 +4032,7 @@
         <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4042,7 +4048,7 @@
         <v>73</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4058,7 +4064,7 @@
         <v>69</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4077,7 +4083,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4093,7 +4099,7 @@
         <v>58</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4109,7 +4115,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4125,7 +4131,7 @@
         <v>65</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4141,7 +4147,7 @@
         <v>60</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4157,7 +4163,7 @@
         <v>62</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4170,10 +4176,10 @@
         <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4184,7 +4190,7 @@
         <v>63</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4200,7 +4206,7 @@
         <v>59</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4216,7 +4222,7 @@
         <v>64</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4229,10 +4235,10 @@
         <v>41</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4243,7 +4249,7 @@
         <v>55</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4259,7 +4265,7 @@
         <v>66</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4275,7 +4281,7 @@
         <v>67</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -4291,17 +4297,17 @@
         <v>63</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,7 +4315,7 @@
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4350,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -4410,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4423,7 +4429,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4439,7 +4445,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4455,7 +4461,7 @@
         <v>76</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4471,7 +4477,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4484,10 +4490,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -4495,7 +4501,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
@@ -4506,7 +4512,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4522,7 +4528,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4538,22 +4544,22 @@
         <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B28" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4719,12 +4725,12 @@
     </row>
     <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4757,7 +4763,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -4823,7 +4829,7 @@
         <v>92</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4839,7 +4845,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4847,10 +4853,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4861,7 +4867,7 @@
         <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -4877,7 +4883,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -4898,7 +4904,7 @@
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4933,14 +4939,14 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="61" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="61"/>
     </row>
     <row r="4" spans="1:5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="59" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
@@ -5004,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5129,7 +5135,7 @@
         <v>109</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5146,7 +5152,7 @@
         <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5183,7 +5189,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -5217,7 +5223,7 @@
         <v>116</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5225,19 +5231,19 @@
     </row>
     <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B36" s="34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B37" s="35" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B38" s="35" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D38" s="5"/>
     </row>
@@ -5247,37 +5253,37 @@
     </row>
     <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B40" s="42" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B43" s="35" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D45" s="5"/>
     </row>
@@ -5313,7 +5319,7 @@
   <sheetData>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -5361,7 +5367,7 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5377,7 +5383,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5385,10 +5391,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5399,7 +5405,7 @@
         <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5415,7 +5421,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5431,7 +5437,7 @@
         <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -5447,12 +5453,12 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B20" s="35" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -5628,7 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -5643,7 +5649,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="56" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -5722,7 +5728,7 @@
         <v>179</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5730,10 +5736,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>411</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5828,7 +5834,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -5920,10 +5926,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5936,13 +5942,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C15" s="53">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -5955,10 +5961,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>403</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>405</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -5971,10 +5977,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="53" t="s">
+        <v>404</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -5990,7 +5996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -6036,7 +6042,7 @@
     <row r="2" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12"/>
       <c r="B2" s="55" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="55"/>
@@ -6068,83 +6074,83 @@
     <row r="3" spans="1:28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="S3" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="T3" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="V3" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="W3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="Z3" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AB3" s="17" t="s">
         <v>311</v>
-      </c>
-      <c r="AA3" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="14.45" x14ac:dyDescent="0.35">
@@ -6185,16 +6191,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -6225,14 +6231,14 @@
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
@@ -6261,7 +6267,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -6269,7 +6275,7 @@
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
@@ -6297,7 +6303,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
@@ -6306,7 +6312,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
       <c r="J8" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -6333,7 +6339,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
@@ -6344,47 +6350,47 @@
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
       <c r="L9" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N9" s="26"/>
       <c r="O9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="W9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z9" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA9" s="26"/>
       <c r="AB9" s="27"/>
@@ -6395,7 +6401,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -6406,7 +6412,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
@@ -6431,7 +6437,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -6443,7 +6449,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
@@ -6467,7 +6473,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -6480,7 +6486,7 @@
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
@@ -6503,7 +6509,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="26"/>
@@ -6517,7 +6523,7 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -6539,7 +6545,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="26"/>
@@ -6554,7 +6560,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -6575,7 +6581,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
@@ -6591,7 +6597,7 @@
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
@@ -6611,7 +6617,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26"/>
@@ -6628,7 +6634,7 @@
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
@@ -6647,7 +6653,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -6665,7 +6671,7 @@
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
       <c r="S17" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -6683,7 +6689,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="26"/>
@@ -6702,10 +6708,10 @@
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U18" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
@@ -6721,7 +6727,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="26"/>
@@ -6741,7 +6747,7 @@
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V19" s="26"/>
       <c r="W19" s="26"/>
@@ -6757,7 +6763,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -6779,7 +6785,7 @@
       <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
@@ -6793,7 +6799,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
@@ -6815,7 +6821,7 @@
       <c r="U21" s="26"/>
       <c r="V21" s="26"/>
       <c r="W21" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
@@ -6829,7 +6835,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="26"/>
@@ -6852,7 +6858,7 @@
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
       <c r="X22" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
@@ -6865,7 +6871,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="26"/>
@@ -6889,13 +6895,13 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AB23" s="27"/>
     </row>
@@ -6905,7 +6911,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -6929,13 +6935,13 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA24" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AB24" s="27"/>
     </row>
@@ -6945,14 +6951,14 @@
         <v>21</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -6981,7 +6987,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="43"/>
@@ -6989,10 +6995,10 @@
       <c r="G26" s="43"/>
       <c r="H26" s="43"/>
       <c r="I26" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="43"/>
@@ -7019,7 +7025,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="43"/>
@@ -7030,7 +7036,7 @@
       <c r="J27" s="43"/>
       <c r="K27" s="43"/>
       <c r="L27" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
@@ -7055,7 +7061,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="43"/>
@@ -7067,29 +7073,29 @@
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U28" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V28" s="43"/>
       <c r="W28" s="43"/>
@@ -7105,7 +7111,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="43"/>
@@ -7127,16 +7133,16 @@
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
       <c r="W29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Y29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Z29" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AA29" s="43"/>
       <c r="AB29" s="27"/>
@@ -7147,13 +7153,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="43"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H30" s="43"/>
       <c r="I30" s="43"/>
@@ -7279,7 +7285,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="26"/>
@@ -7287,7 +7293,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
@@ -7303,7 +7309,7 @@
       <c r="U34" s="26"/>
       <c r="V34" s="26"/>
       <c r="W34" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="X34" s="26"/>
       <c r="Y34" s="26"/>
@@ -7317,7 +7323,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="26"/>
@@ -7326,7 +7332,7 @@
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
@@ -7353,7 +7359,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="26"/>
@@ -7365,17 +7371,17 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="Q36" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="R36" s="26"/>
       <c r="S36" s="26"/>
@@ -7395,7 +7401,7 @@
         <v>33</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="26"/>
@@ -7412,19 +7418,19 @@
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
       <c r="R37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="S37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="T37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="V37" s="26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
@@ -7597,7 +7603,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="48" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -7636,180 +7642,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="56" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-    </row>
-    <row r="4" spans="1:4" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>205</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
@@ -7826,7 +7658,7 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
@@ -7966,7 +7798,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8103,6 +7935,188 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="63" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>415</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -8116,7 +8130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
@@ -8133,7 +8147,7 @@
     </row>
     <row r="3" spans="1:4" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -8195,10 +8209,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8212,10 +8226,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8229,10 +8243,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8246,10 +8260,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -8282,7 +8296,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -8456,7 +8470,7 @@
         <v>140</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8476,7 +8490,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8496,7 +8510,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8558,7 +8572,7 @@
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B34" s="40" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -8592,7 +8606,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="17.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="56" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
@@ -8661,7 +8675,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8680,7 +8694,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8699,7 +8713,7 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8715,7 +8729,7 @@
         <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" x14ac:dyDescent="0.35">
@@ -8768,7 +8782,7 @@
     </row>
     <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B24" s="41" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -8925,7 +8939,7 @@
         <v>158</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -8954,10 +8968,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -9095,7 +9109,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
@@ -9159,7 +9173,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D20" t="s">
         <v>160</v>
@@ -9804,17 +9818,17 @@
     </row>
     <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B47" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="35" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -10190,12 +10204,12 @@
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="37" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -10562,17 +10576,17 @@
     </row>
     <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B48" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B49" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -10664,13 +10678,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C10" s="49">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10686,13 +10700,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C12" s="49">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10708,13 +10722,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C14" s="49">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10730,11 +10744,11 @@
         <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -10750,11 +10764,11 @@
         <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10959,7 +10973,7 @@
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
@@ -10993,12 +11007,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -11118,12 +11132,12 @@
     </row>
     <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B16" s="35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -11227,7 +11241,7 @@
     </row>
     <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B14" s="35" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>